<commit_message>
Add files for PCB bringup.
Update FPGA image with 3.3V I/O logic (counter bound to I/O pins).
</commit_message>
<xml_diff>
--- a/05-verification/Problem Report Status.xlsx
+++ b/05-verification/Problem Report Status.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Korwinula\Documents\MIDI-Router\05-verification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BD1BFDF2-101A-4F52-A18D-B0C39C9C12E9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4E92E1C1-45E3-4B86-9A6B-32B34C8229DD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" xr2:uid="{01F44502-D890-40F0-99CD-8DF1ED07B517}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Problem Report</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>PCB</t>
+  </si>
+  <si>
+    <t>PR-003</t>
+  </si>
+  <si>
+    <t>Software-app</t>
   </si>
 </sst>
 </file>
@@ -407,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70E0E73-8351-4979-AE3E-866C8A049AC7}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -475,6 +481,20 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>43343</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add files for PCB releases.
</commit_message>
<xml_diff>
--- a/05-verification/Problem Report Status.xlsx
+++ b/05-verification/Problem Report Status.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Korwinula\Documents\MIDI-Router\05-verification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kander4\Documents\MIDI-Router\05-verification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4E92E1C1-45E3-4B86-9A6B-32B34C8229DD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F362C3-BA47-4C31-ADA0-B3FC69AD4C00}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" xr2:uid="{01F44502-D890-40F0-99CD-8DF1ED07B517}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{01F44502-D890-40F0-99CD-8DF1ED07B517}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Problem Report</t>
   </si>
@@ -61,6 +61,48 @@
   </si>
   <si>
     <t>Software-app</t>
+  </si>
+  <si>
+    <t>PR-004</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>MCU hardware pin is not able to drive the MODE LED</t>
+  </si>
+  <si>
+    <t>MCU hardware pin is not able to drive the CRESET pin</t>
+  </si>
+  <si>
+    <t>Software defect results in MCU firmware lockup</t>
+  </si>
+  <si>
+    <t>FPGA is not able to drive MIDI THRU signals</t>
+  </si>
+  <si>
+    <t>MCU is not able to drive SCL/SDA signals. See PR-004</t>
+  </si>
+  <si>
+    <t>PR-005</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>PCB - MODE LED</t>
+  </si>
+  <si>
+    <t>PCB - CRESET</t>
+  </si>
+  <si>
+    <t>SW - USB CDC Lockup</t>
+  </si>
+  <si>
+    <t>FW - MIDI THRU</t>
+  </si>
+  <si>
+    <t>PCB - I2C</t>
   </si>
 </sst>
 </file>
@@ -413,21 +455,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70E0E73-8351-4979-AE3E-866C8A049AC7}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -446,8 +489,14 @@
       <c r="F1" t="s">
         <v>8</v>
       </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43231</v>
       </c>
@@ -463,8 +512,14 @@
       <c r="F2" t="s">
         <v>9</v>
       </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43231</v>
       </c>
@@ -480,11 +535,20 @@
       <c r="F3" t="s">
         <v>9</v>
       </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43343</v>
       </c>
+      <c r="B4" s="1">
+        <v>43558</v>
+      </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
@@ -493,6 +557,52 @@
       </c>
       <c r="F4" t="s">
         <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43558</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>43558</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>